<commit_message>
ASLCaserta - Errato commit precedente
Effettuata nuova commit per errato posizionamento dei files
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#150203000000XX/ASL_Caserta/ASLCE_ADTPS/1.0/report-checklist.xlsx
+++ b/GATEWAY/A1#150203000000XX/ASL_Caserta/ASLCE_ADTPS/1.0/report-checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dario.sommonte\Documents\DOCUMENTI UFFICIO\FSE-CDA2\AGGIORNAMENTO FSE2\ACCREDITAMENTO\GATEWAY\A1#150203000000XX\ASL_Caserta\ASLCE_ADTPS\1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1289080-62D9-40F1-ADC9-554F2576BF54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E129392C-5AA6-41E9-9F16-952B7801A804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30" yWindow="630" windowWidth="28770" windowHeight="15570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="3" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="306">
   <si>
     <t>NOME FORNITORE:</t>
   </si>
@@ -822,334 +822,409 @@
     <t>L’errore si può verificare solo in caso di cambio di specifiche di generazione di token</t>
   </si>
   <si>
-    <t>11/04/2023</t>
-  </si>
-  <si>
-    <t>11/04/2023 11:56:02</t>
-  </si>
-  <si>
-    <t>54cddfff5c17e7ef</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.e883906759350f874e146c909b921a54c8d82a646997feb46ad26be1982458a2.4709fab583^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>11/04/2023 00:31:48</t>
-  </si>
-  <si>
-    <t>f46a515a386c2ec9</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.e883906759350f874e146c909b921a54c8d82a646997feb46ad26be1982458a2.39e7e0985a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>11/04/2023 01:30:33</t>
-  </si>
-  <si>
-    <t>ffb10b06d321cff6</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.e883906759350f874e146c909b921a54c8d82a646997feb46ad26be1982458a2.d7bbd04e57^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>11/04/2023 03:50:55</t>
-  </si>
-  <si>
-    <t>91bd887ebbb7ec35</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.e883906759350f874e146c909b921a54c8d82a646997feb46ad26be1982458a2.8d7cfcb1a5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>11/04/2023 03:53:02</t>
-  </si>
-  <si>
-    <t>2d351896df406797</t>
-  </si>
-  <si>
-    <t>11/04/2023 03:53:04</t>
-  </si>
-  <si>
-    <t>c7ccdb54f5fe8c27</t>
-  </si>
-  <si>
-    <t>11/04/2023 03:52:35</t>
-  </si>
-  <si>
-    <t>a0d67038814bc938</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.e883906759350f874e146c909b921a54c8d82a646997feb46ad26be1982458a2.71c65f3e12^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>12/04/2023</t>
-  </si>
-  <si>
-    <t>12/04/2023 00:00:24</t>
-  </si>
-  <si>
-    <t>e1de3b45bde96a7e</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.05749625b2397823fb6e622bd34c86f95d4204a8d88eda08af3467630d91b2bd.76766ad8fe^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>12/04/2023 01:34:10</t>
-  </si>
-  <si>
-    <t>1167e24d940d0502</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.05749625b2397823fb6e622bd34c86f95d4204a8d88eda08af3467630d91b2bd.1162de550b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>13/04/2023</t>
-  </si>
-  <si>
-    <t>13/04/2023 01:13:14</t>
-  </si>
-  <si>
-    <t>268e0f985dced490</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.05749625b2397823fb6e622bd34c86f95d4204a8d88eda08af3467630d91b2bd.411b21be51^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>13/04/2023 02:31:02</t>
-  </si>
-  <si>
-    <t>4ab9d58415552d3a</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.05749625b2397823fb6e622bd34c86f95d4204a8d88eda08af3467630d91b2bd.0e8e96cf26^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>13/04/2023 02:33:38</t>
-  </si>
-  <si>
-    <t>04349edf7e685346</t>
-  </si>
-  <si>
-    <t>13/04/2023 02:32:29</t>
-  </si>
-  <si>
-    <t>dfab4ef46c36ba86</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.05749625b2397823fb6e622bd34c86f95d4204a8d88eda08af3467630d91b2bd.f1dd2f8a16^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>13/04/2023 02:32:32</t>
-  </si>
-  <si>
-    <t>9825937a181d8da0</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.05749625b2397823fb6e622bd34c86f95d4204a8d88eda08af3467630d91b2bd.e2466c96ba^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>13/04/2023 02:32:34</t>
-  </si>
-  <si>
-    <t>6dacd436f1a923f8</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.05749625b2397823fb6e622bd34c86f95d4204a8d88eda08af3467630d91b2bd.71d3bee196^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>13/04/2023 02:32:36</t>
-  </si>
-  <si>
-    <t>ee48d2124be7386d</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.05749625b2397823fb6e622bd34c86f95d4204a8d88eda08af3467630d91b2bd.f39ab9c4ad^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>13/04/2023 02:32:38</t>
-  </si>
-  <si>
-    <t>c3948bcf13e16bcd</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.05749625b2397823fb6e622bd34c86f95d4204a8d88eda08af3467630d91b2bd.bdbc3e8adf^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>13/04/2023 02:32:41</t>
-  </si>
-  <si>
-    <t>54ad7ffb7c225f68</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.05749625b2397823fb6e622bd34c86f95d4204a8d88eda08af3467630d91b2bd.6a606af68f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>13/04/2023 02:32:44</t>
-  </si>
-  <si>
-    <t>b8aebb008e403569</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.05749625b2397823fb6e622bd34c86f95d4204a8d88eda08af3467630d91b2bd.2b7add8349^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>13/04/2023 02:32:46</t>
-  </si>
-  <si>
-    <t>188fb87f63aacb3c</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.05749625b2397823fb6e622bd34c86f95d4204a8d88eda08af3467630d91b2bd.cf4b2569db^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>13/04/2023 02:32:49</t>
-  </si>
-  <si>
-    <t>77c6915c50dbc8a8</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.05749625b2397823fb6e622bd34c86f95d4204a8d88eda08af3467630d91b2bd.f49b8b021c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>13/04/2023 02:32:52</t>
-  </si>
-  <si>
-    <t>e116ec70efac13f3</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.05749625b2397823fb6e622bd34c86f95d4204a8d88eda08af3467630d91b2bd.47c81a9e73^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>13/04/2023 02:32:54</t>
-  </si>
-  <si>
-    <t>b0dca0b0761deb8e</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.05749625b2397823fb6e622bd34c86f95d4204a8d88eda08af3467630d91b2bd.dfbba511d5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>13/04/2023 02:32:56</t>
-  </si>
-  <si>
-    <t>eb0173d1cfc66ddd</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.05749625b2397823fb6e622bd34c86f95d4204a8d88eda08af3467630d91b2bd.f77926ecf8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>13/04/2023 02:32:59</t>
-  </si>
-  <si>
-    <t>fc2d831e2a772225</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.05749625b2397823fb6e622bd34c86f95d4204a8d88eda08af3467630d91b2bd.01ee0075f5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>13/04/2023 02:33:01</t>
-  </si>
-  <si>
-    <t>cb671a93f0634f23</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.05749625b2397823fb6e622bd34c86f95d4204a8d88eda08af3467630d91b2bd.d370feeb6a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>13/04/2023 02:33:03</t>
-  </si>
-  <si>
-    <t>d7e49a2bb584db95</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.05749625b2397823fb6e622bd34c86f95d4204a8d88eda08af3467630d91b2bd.09418781d8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>13/04/2023 02:33:05</t>
-  </si>
-  <si>
-    <t>181020fce06c7fd6</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.05749625b2397823fb6e622bd34c86f95d4204a8d88eda08af3467630d91b2bd.57a90ec5a4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>13/04/2023 02:33:08</t>
-  </si>
-  <si>
-    <t>e75e7c30586b595f</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.05749625b2397823fb6e622bd34c86f95d4204a8d88eda08af3467630d91b2bd.a4aa267e98^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>13/04/2023 02:33:10</t>
-  </si>
-  <si>
-    <t>6053b8a4c5a31c59</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.05749625b2397823fb6e622bd34c86f95d4204a8d88eda08af3467630d91b2bd.f640d1a381^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>13/04/2023 02:33:12</t>
-  </si>
-  <si>
-    <t>f3e07b03249e7730</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.05749625b2397823fb6e622bd34c86f95d4204a8d88eda08af3467630d91b2bd.d71e5a93e9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>13/04/2023 02:33:15</t>
-  </si>
-  <si>
-    <t>2404b37d91de3da3</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.05749625b2397823fb6e622bd34c86f95d4204a8d88eda08af3467630d91b2bd.b698b519b3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>13/04/2023 02:33:17</t>
-  </si>
-  <si>
-    <t>88dd88618039f4f4</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.05749625b2397823fb6e622bd34c86f95d4204a8d88eda08af3467630d91b2bd.77c22389b2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>13/04/2023 02:33:22</t>
-  </si>
-  <si>
-    <t>8822634a05a11bed</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.05749625b2397823fb6e622bd34c86f95d4204a8d88eda08af3467630d91b2bd.488a842062^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>13/04/2023 02:33:26</t>
-  </si>
-  <si>
-    <t>20f53c7a697df124</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.05749625b2397823fb6e622bd34c86f95d4204a8d88eda08af3467630d91b2bd.7ca4d2bbbf^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>13/04/2023 02:33:30</t>
-  </si>
-  <si>
-    <t>d7419788cac99fdf</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.05749625b2397823fb6e622bd34c86f95d4204a8d88eda08af3467630d91b2bd.449e062ee7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>13/04/2023 02:51:14</t>
-  </si>
-  <si>
-    <t>ad08b95c96db43a9</t>
+    <t>18/04/2023</t>
+  </si>
+  <si>
+    <t>18/04/2023 02:26:29</t>
+  </si>
+  <si>
+    <t>7c3e5963882bf0a8</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.e883906759350f874e146c909b921a54c8d82a646997feb46ad26be1982458a2.8e8514661a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>18/04/2023 02:26:32</t>
+  </si>
+  <si>
+    <t>7d978bce40c20f72</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.e883906759350f874e146c909b921a54c8d82a646997feb46ad26be1982458a2.04ae1a81f3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>18/04/2023 02:26:35</t>
+  </si>
+  <si>
+    <t>160bfa962f2874a6</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.e883906759350f874e146c909b921a54c8d82a646997feb46ad26be1982458a2.7179fe8f12^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>18/04/2023 02:26:37</t>
+  </si>
+  <si>
+    <t>cc27a1299a3f0fe1</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.e883906759350f874e146c909b921a54c8d82a646997feb46ad26be1982458a2.76f061f0bf^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>18/04/2023 02:24:56</t>
+  </si>
+  <si>
+    <t>0fc88a0b96a2bfd4</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.05749625b2397823fb6e622bd34c86f95d4204a8d88eda08af3467630d91b2bd.1f6d5429a6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>18/04/2023 02:24:59</t>
+  </si>
+  <si>
+    <t>b1e83066d95c4b7d</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.05749625b2397823fb6e622bd34c86f95d4204a8d88eda08af3467630d91b2bd.e2000b05b5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>18/04/2023 02:25:01</t>
+  </si>
+  <si>
+    <t>b5b327df15660c4a</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.05749625b2397823fb6e622bd34c86f95d4204a8d88eda08af3467630d91b2bd.2eff41cf5b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>18/04/2023 02:25:04</t>
+  </si>
+  <si>
+    <t>759dfbf90b48fb62</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.05749625b2397823fb6e622bd34c86f95d4204a8d88eda08af3467630d91b2bd.e254e75390^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>18/04/2023 02:27:07</t>
+  </si>
+  <si>
+    <t>cd73a73a3f86ff19</t>
+  </si>
+  <si>
+    <t>18/04/2023 02:26:24</t>
+  </si>
+  <si>
+    <t>6691efc8f329a433</t>
+  </si>
+  <si>
+    <t>18/04/2023 02:27:13</t>
+  </si>
+  <si>
+    <t>0fb717dd03b12646</t>
+  </si>
+  <si>
+    <t>18/04/2023 02:26:26</t>
+  </si>
+  <si>
+    <t>1be4693140518dc2</t>
+  </si>
+  <si>
+    <t>18/04/2023 02:26:40</t>
+  </si>
+  <si>
+    <t>995b3a4048f56911</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.e883906759350f874e146c909b921a54c8d82a646997feb46ad26be1982458a2.5f99f0dbb2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>18/04/2023 02:26:42</t>
+  </si>
+  <si>
+    <t>3faaf97bb47479c0</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.e883906759350f874e146c909b921a54c8d82a646997feb46ad26be1982458a2.648844608b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>18/04/2023 02:26:45</t>
+  </si>
+  <si>
+    <t>94ce2ac31869c8c3</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.e883906759350f874e146c909b921a54c8d82a646997feb46ad26be1982458a2.71b06f50d6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>18/04/2023 02:26:47</t>
+  </si>
+  <si>
+    <t>cdd8c96a0e0a1a1a</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.e883906759350f874e146c909b921a54c8d82a646997feb46ad26be1982458a2.2658463ced^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>18/04/2023 02:26:51</t>
+  </si>
+  <si>
+    <t>0ea713d0056944c9</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.e883906759350f874e146c909b921a54c8d82a646997feb46ad26be1982458a2.059c911179^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>18/04/2023 02:26:53</t>
+  </si>
+  <si>
+    <t>4e341843397d917b</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.e883906759350f874e146c909b921a54c8d82a646997feb46ad26be1982458a2.c74fd9972c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>18/04/2023 02:26:56</t>
+  </si>
+  <si>
+    <t>d359f91842537fa1</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.e883906759350f874e146c909b921a54c8d82a646997feb46ad26be1982458a2.0fa2797dce^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>18/04/2023 02:26:58</t>
+  </si>
+  <si>
+    <t>3c2e18953ca1039f</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.e883906759350f874e146c909b921a54c8d82a646997feb46ad26be1982458a2.5d7f71f85a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>18/04/2023 02:27:01</t>
+  </si>
+  <si>
+    <t>2f143c8db4714910</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.e883906759350f874e146c909b921a54c8d82a646997feb46ad26be1982458a2.10ed52b182^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>18/04/2023 02:27:04</t>
+  </si>
+  <si>
+    <t>d450358b15f42d5a</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.e883906759350f874e146c909b921a54c8d82a646997feb46ad26be1982458a2.f01e5d4b9e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>18/04/2023 02:25:07</t>
+  </si>
+  <si>
+    <t>45aa58abe73d74ce</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.05749625b2397823fb6e622bd34c86f95d4204a8d88eda08af3467630d91b2bd.40e5516f77^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>18/04/2023 02:25:13</t>
+  </si>
+  <si>
+    <t>70a2b35b2be236af</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.05749625b2397823fb6e622bd34c86f95d4204a8d88eda08af3467630d91b2bd.b1e8faaae5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>18/04/2023 02:25:16</t>
+  </si>
+  <si>
+    <t>aea426a07fe0c28d</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.05749625b2397823fb6e622bd34c86f95d4204a8d88eda08af3467630d91b2bd.8276916eb9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>18/04/2023 02:25:18</t>
+  </si>
+  <si>
+    <t>5c1afb00d3b5c0b5</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.05749625b2397823fb6e622bd34c86f95d4204a8d88eda08af3467630d91b2bd.e05cc9c04c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>18/04/2023 02:25:21</t>
+  </si>
+  <si>
+    <t>433d3769d30fc808</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.05749625b2397823fb6e622bd34c86f95d4204a8d88eda08af3467630d91b2bd.b7e446d242^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>18/04/2023 02:25:24</t>
+  </si>
+  <si>
+    <t>01f4f6f24f46ca1a</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.05749625b2397823fb6e622bd34c86f95d4204a8d88eda08af3467630d91b2bd.d59af4f6a1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>18/04/2023 02:25:26</t>
+  </si>
+  <si>
+    <t>0f7d2203e9090120</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.05749625b2397823fb6e622bd34c86f95d4204a8d88eda08af3467630d91b2bd.b66d83b0d4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>18/04/2023 02:25:29</t>
+  </si>
+  <si>
+    <t>69a464ce643392e3</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.05749625b2397823fb6e622bd34c86f95d4204a8d88eda08af3467630d91b2bd.e05882c107^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>18/04/2023 02:25:32</t>
+  </si>
+  <si>
+    <t>1a23e82ed002466b</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.05749625b2397823fb6e622bd34c86f95d4204a8d88eda08af3467630d91b2bd.ae996f4595^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>18/04/2023 02:25:39</t>
+  </si>
+  <si>
+    <t>6e4ac6b273e93f59</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.05749625b2397823fb6e622bd34c86f95d4204a8d88eda08af3467630d91b2bd.1f4c45ddea^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>18/04/2023 02:25:42</t>
+  </si>
+  <si>
+    <t>c359782383da95ad</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.05749625b2397823fb6e622bd34c86f95d4204a8d88eda08af3467630d91b2bd.699b4c7aea^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>18/04/2023 02:25:45</t>
+  </si>
+  <si>
+    <t>169000e8ca8a91ba</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.05749625b2397823fb6e622bd34c86f95d4204a8d88eda08af3467630d91b2bd.2b8247e090^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>18/04/2023 02:25:48</t>
+  </si>
+  <si>
+    <t>6f870121cd403f8b</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.05749625b2397823fb6e622bd34c86f95d4204a8d88eda08af3467630d91b2bd.ef15b98aa5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>18/04/2023 02:25:50</t>
+  </si>
+  <si>
+    <t>e4c4451419020fdf</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.05749625b2397823fb6e622bd34c86f95d4204a8d88eda08af3467630d91b2bd.63442d98a9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>18/04/2023 02:25:53</t>
+  </si>
+  <si>
+    <t>923f2d7bffc67a2b</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.05749625b2397823fb6e622bd34c86f95d4204a8d88eda08af3467630d91b2bd.c578f27813^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>18/04/2023 02:25:55</t>
+  </si>
+  <si>
+    <t>20caa40a5ba71c78</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.05749625b2397823fb6e622bd34c86f95d4204a8d88eda08af3467630d91b2bd.96e8b6cf46^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>18/04/2023 02:25:59</t>
+  </si>
+  <si>
+    <t>a00c58f178e30daf</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.05749625b2397823fb6e622bd34c86f95d4204a8d88eda08af3467630d91b2bd.5a2fc508ce^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>18/04/2023 02:26:03</t>
+  </si>
+  <si>
+    <t>0377e7e31dd94f77</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.05749625b2397823fb6e622bd34c86f95d4204a8d88eda08af3467630d91b2bd.94b1186b29^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>18/04/2023 02:26:08</t>
+  </si>
+  <si>
+    <t>8b5585d3d4985efd</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.05749625b2397823fb6e622bd34c86f95d4204a8d88eda08af3467630d91b2bd.aeab20db06^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>18/04/2023 02:26:11</t>
+  </si>
+  <si>
+    <t>0ed3c7a6f8d4c4a5</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.05749625b2397823fb6e622bd34c86f95d4204a8d88eda08af3467630d91b2bd.62d9d4ca13^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>18/04/2023 02:26:14</t>
+  </si>
+  <si>
+    <t>d11a11feb9af0ec7</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.05749625b2397823fb6e622bd34c86f95d4204a8d88eda08af3467630d91b2bd.a6b4ba5ce1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>18/04/2023 02:26:17</t>
+  </si>
+  <si>
+    <t>5de2a7fc736315f9</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.05749625b2397823fb6e622bd34c86f95d4204a8d88eda08af3467630d91b2bd.904d5b74d2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>18/04/2023 02:26:19</t>
+  </si>
+  <si>
+    <t>7da4cf147d0ffc05</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.05749625b2397823fb6e622bd34c86f95d4204a8d88eda08af3467630d91b2bd.f0517e623b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>18/04/2023 02:26:22</t>
+  </si>
+  <si>
+    <t>6161b033763ec183</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.05749625b2397823fb6e622bd34c86f95d4204a8d88eda08af3467630d91b2bd.32b6742cb5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -1794,7 +1869,7 @@
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomRight" activeCell="F55" sqref="F55:I60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2257,16 +2332,16 @@
         <v>36</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="I14" s="14" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="J14" s="20" t="s">
         <v>52</v>
@@ -2305,16 +2380,16 @@
         <v>38</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
       <c r="G15" s="14" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="H15" s="14" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="J15" s="20" t="s">
         <v>52</v>
@@ -2353,16 +2428,16 @@
         <v>40</v>
       </c>
       <c r="F16" s="13" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="I16" s="14" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="J16" s="20" t="s">
         <v>52</v>
@@ -2401,16 +2476,16 @@
         <v>42</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="G17" s="14" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="H17" s="14" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="I17" s="14" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="J17" s="20" t="s">
         <v>52</v>
@@ -2452,10 +2527,10 @@
         <v>171</v>
       </c>
       <c r="G18" s="14" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="H18" s="14" t="s">
-        <v>185</v>
+        <v>197</v>
       </c>
       <c r="I18" s="14" t="s">
         <v>136</v>
@@ -2508,10 +2583,10 @@
         <v>171</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>186</v>
+        <v>198</v>
       </c>
       <c r="H19" s="14" t="s">
-        <v>187</v>
+        <v>199</v>
       </c>
       <c r="I19" s="14" t="s">
         <v>136</v>
@@ -2561,13 +2636,13 @@
         <v>48</v>
       </c>
       <c r="F20" s="13" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>279</v>
+        <v>200</v>
       </c>
       <c r="H20" s="14" t="s">
-        <v>280</v>
+        <v>201</v>
       </c>
       <c r="I20" s="14" t="s">
         <v>136</v>
@@ -2617,13 +2692,13 @@
         <v>50</v>
       </c>
       <c r="F21" s="13" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="G21" s="14" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="H21" s="14" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="I21" s="14" t="s">
         <v>136</v>
@@ -2752,13 +2827,13 @@
         <v>171</v>
       </c>
       <c r="G24" s="14" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="H24" s="14" t="s">
-        <v>189</v>
+        <v>205</v>
       </c>
       <c r="I24" s="14" t="s">
-        <v>190</v>
+        <v>206</v>
       </c>
       <c r="J24" s="15" t="s">
         <v>52</v>
@@ -2844,13 +2919,13 @@
         <v>171</v>
       </c>
       <c r="G26" s="14" t="s">
-        <v>188</v>
+        <v>207</v>
       </c>
       <c r="H26" s="14" t="s">
-        <v>189</v>
+        <v>208</v>
       </c>
       <c r="I26" s="14" t="s">
-        <v>190</v>
+        <v>209</v>
       </c>
       <c r="J26" s="15" t="s">
         <v>52</v>
@@ -2898,13 +2973,13 @@
         <v>171</v>
       </c>
       <c r="G27" s="14" t="s">
-        <v>188</v>
+        <v>210</v>
       </c>
       <c r="H27" s="14" t="s">
-        <v>189</v>
+        <v>211</v>
       </c>
       <c r="I27" s="14" t="s">
-        <v>190</v>
+        <v>212</v>
       </c>
       <c r="J27" s="15" t="s">
         <v>52</v>
@@ -2952,13 +3027,13 @@
         <v>171</v>
       </c>
       <c r="G28" s="14" t="s">
-        <v>188</v>
+        <v>213</v>
       </c>
       <c r="H28" s="14" t="s">
-        <v>189</v>
+        <v>214</v>
       </c>
       <c r="I28" s="14" t="s">
-        <v>190</v>
+        <v>215</v>
       </c>
       <c r="J28" s="15" t="s">
         <v>52</v>
@@ -3006,13 +3081,13 @@
         <v>171</v>
       </c>
       <c r="G29" s="14" t="s">
-        <v>188</v>
+        <v>216</v>
       </c>
       <c r="H29" s="14" t="s">
-        <v>189</v>
+        <v>217</v>
       </c>
       <c r="I29" s="14" t="s">
-        <v>190</v>
+        <v>218</v>
       </c>
       <c r="J29" s="15" t="s">
         <v>52</v>
@@ -3060,13 +3135,13 @@
         <v>171</v>
       </c>
       <c r="G30" s="14" t="s">
-        <v>188</v>
+        <v>219</v>
       </c>
       <c r="H30" s="14" t="s">
-        <v>189</v>
+        <v>220</v>
       </c>
       <c r="I30" s="14" t="s">
-        <v>190</v>
+        <v>221</v>
       </c>
       <c r="J30" s="15" t="s">
         <v>52</v>
@@ -3114,13 +3189,13 @@
         <v>171</v>
       </c>
       <c r="G31" s="14" t="s">
-        <v>188</v>
+        <v>222</v>
       </c>
       <c r="H31" s="14" t="s">
-        <v>189</v>
+        <v>223</v>
       </c>
       <c r="I31" s="14" t="s">
-        <v>190</v>
+        <v>224</v>
       </c>
       <c r="J31" s="15" t="s">
         <v>52</v>
@@ -3168,13 +3243,13 @@
         <v>171</v>
       </c>
       <c r="G32" s="14" t="s">
-        <v>188</v>
+        <v>225</v>
       </c>
       <c r="H32" s="14" t="s">
-        <v>189</v>
+        <v>226</v>
       </c>
       <c r="I32" s="14" t="s">
-        <v>190</v>
+        <v>227</v>
       </c>
       <c r="J32" s="15" t="s">
         <v>52</v>
@@ -3222,13 +3297,13 @@
         <v>171</v>
       </c>
       <c r="G33" s="14" t="s">
-        <v>188</v>
+        <v>228</v>
       </c>
       <c r="H33" s="14" t="s">
-        <v>189</v>
+        <v>229</v>
       </c>
       <c r="I33" s="14" t="s">
-        <v>190</v>
+        <v>230</v>
       </c>
       <c r="J33" s="15" t="s">
         <v>52</v>
@@ -3276,13 +3351,13 @@
         <v>171</v>
       </c>
       <c r="G34" s="14" t="s">
-        <v>188</v>
+        <v>231</v>
       </c>
       <c r="H34" s="14" t="s">
-        <v>189</v>
+        <v>232</v>
       </c>
       <c r="I34" s="14" t="s">
-        <v>190</v>
+        <v>233</v>
       </c>
       <c r="J34" s="15" t="s">
         <v>52</v>
@@ -3365,16 +3440,16 @@
         <v>80</v>
       </c>
       <c r="F36" s="13" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="G36" s="14" t="s">
-        <v>207</v>
+        <v>234</v>
       </c>
       <c r="H36" s="14" t="s">
-        <v>208</v>
+        <v>235</v>
       </c>
       <c r="I36" s="14" t="s">
-        <v>209</v>
+        <v>236</v>
       </c>
       <c r="J36" s="15" t="s">
         <v>52</v>
@@ -3457,16 +3532,16 @@
         <v>84</v>
       </c>
       <c r="F38" s="13" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="G38" s="14" t="s">
-        <v>210</v>
+        <v>237</v>
       </c>
       <c r="H38" s="14" t="s">
-        <v>211</v>
+        <v>238</v>
       </c>
       <c r="I38" s="14" t="s">
-        <v>212</v>
+        <v>239</v>
       </c>
       <c r="J38" s="15" t="s">
         <v>52</v>
@@ -3511,16 +3586,16 @@
         <v>86</v>
       </c>
       <c r="F39" s="13" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="G39" s="14" t="s">
-        <v>213</v>
+        <v>240</v>
       </c>
       <c r="H39" s="14" t="s">
-        <v>214</v>
+        <v>241</v>
       </c>
       <c r="I39" s="14" t="s">
-        <v>215</v>
+        <v>242</v>
       </c>
       <c r="J39" s="15" t="s">
         <v>52</v>
@@ -3565,16 +3640,16 @@
         <v>88</v>
       </c>
       <c r="F40" s="13" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="G40" s="14" t="s">
-        <v>216</v>
+        <v>243</v>
       </c>
       <c r="H40" s="14" t="s">
-        <v>217</v>
+        <v>244</v>
       </c>
       <c r="I40" s="14" t="s">
-        <v>218</v>
+        <v>245</v>
       </c>
       <c r="J40" s="15" t="s">
         <v>52</v>
@@ -3619,16 +3694,16 @@
         <v>90</v>
       </c>
       <c r="F41" s="13" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="G41" s="14" t="s">
-        <v>219</v>
+        <v>246</v>
       </c>
       <c r="H41" s="14" t="s">
-        <v>220</v>
+        <v>247</v>
       </c>
       <c r="I41" s="14" t="s">
-        <v>221</v>
+        <v>248</v>
       </c>
       <c r="J41" s="15" t="s">
         <v>52</v>
@@ -3673,16 +3748,16 @@
         <v>92</v>
       </c>
       <c r="F42" s="13" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="G42" s="14" t="s">
-        <v>222</v>
+        <v>249</v>
       </c>
       <c r="H42" s="14" t="s">
-        <v>223</v>
+        <v>250</v>
       </c>
       <c r="I42" s="14" t="s">
-        <v>224</v>
+        <v>251</v>
       </c>
       <c r="J42" s="15" t="s">
         <v>52</v>
@@ -3727,16 +3802,16 @@
         <v>94</v>
       </c>
       <c r="F43" s="13" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="G43" s="14" t="s">
-        <v>225</v>
+        <v>252</v>
       </c>
       <c r="H43" s="14" t="s">
-        <v>226</v>
+        <v>253</v>
       </c>
       <c r="I43" s="14" t="s">
-        <v>227</v>
+        <v>254</v>
       </c>
       <c r="J43" s="15" t="s">
         <v>52</v>
@@ -3781,16 +3856,16 @@
         <v>96</v>
       </c>
       <c r="F44" s="13" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="G44" s="14" t="s">
-        <v>228</v>
+        <v>255</v>
       </c>
       <c r="H44" s="14" t="s">
-        <v>229</v>
+        <v>256</v>
       </c>
       <c r="I44" s="14" t="s">
-        <v>230</v>
+        <v>257</v>
       </c>
       <c r="J44" s="15" t="s">
         <v>52</v>
@@ -3835,16 +3910,16 @@
         <v>98</v>
       </c>
       <c r="F45" s="13" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="G45" s="14" t="s">
-        <v>231</v>
+        <v>258</v>
       </c>
       <c r="H45" s="14" t="s">
-        <v>232</v>
+        <v>259</v>
       </c>
       <c r="I45" s="14" t="s">
-        <v>233</v>
+        <v>260</v>
       </c>
       <c r="J45" s="15" t="s">
         <v>52</v>
@@ -3889,16 +3964,16 @@
         <v>100</v>
       </c>
       <c r="F46" s="13" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="G46" s="14" t="s">
-        <v>234</v>
+        <v>261</v>
       </c>
       <c r="H46" s="14" t="s">
-        <v>235</v>
+        <v>262</v>
       </c>
       <c r="I46" s="14" t="s">
-        <v>236</v>
+        <v>263</v>
       </c>
       <c r="J46" s="15" t="s">
         <v>52</v>
@@ -3943,16 +4018,16 @@
         <v>102</v>
       </c>
       <c r="F47" s="13" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="G47" s="14" t="s">
-        <v>237</v>
+        <v>264</v>
       </c>
       <c r="H47" s="14" t="s">
-        <v>238</v>
+        <v>265</v>
       </c>
       <c r="I47" s="14" t="s">
-        <v>239</v>
+        <v>266</v>
       </c>
       <c r="J47" s="15" t="s">
         <v>52</v>
@@ -3997,16 +4072,16 @@
         <v>104</v>
       </c>
       <c r="F48" s="13" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="G48" s="14" t="s">
-        <v>240</v>
+        <v>267</v>
       </c>
       <c r="H48" s="14" t="s">
-        <v>241</v>
+        <v>268</v>
       </c>
       <c r="I48" s="14" t="s">
-        <v>242</v>
+        <v>269</v>
       </c>
       <c r="J48" s="15" t="s">
         <v>52</v>
@@ -4051,16 +4126,16 @@
         <v>106</v>
       </c>
       <c r="F49" s="13" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="G49" s="14" t="s">
-        <v>243</v>
+        <v>270</v>
       </c>
       <c r="H49" s="14" t="s">
-        <v>244</v>
+        <v>271</v>
       </c>
       <c r="I49" s="14" t="s">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="J49" s="15" t="s">
         <v>52</v>
@@ -4105,16 +4180,16 @@
         <v>108</v>
       </c>
       <c r="F50" s="13" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="G50" s="14" t="s">
-        <v>246</v>
+        <v>273</v>
       </c>
       <c r="H50" s="14" t="s">
-        <v>247</v>
+        <v>274</v>
       </c>
       <c r="I50" s="14" t="s">
-        <v>248</v>
+        <v>275</v>
       </c>
       <c r="J50" s="15" t="s">
         <v>52</v>
@@ -4159,16 +4234,16 @@
         <v>110</v>
       </c>
       <c r="F51" s="13" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="G51" s="14" t="s">
-        <v>249</v>
+        <v>276</v>
       </c>
       <c r="H51" s="14" t="s">
-        <v>250</v>
+        <v>277</v>
       </c>
       <c r="I51" s="14" t="s">
-        <v>251</v>
+        <v>278</v>
       </c>
       <c r="J51" s="15" t="s">
         <v>52</v>
@@ -4213,16 +4288,16 @@
         <v>112</v>
       </c>
       <c r="F52" s="13" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="G52" s="14" t="s">
-        <v>252</v>
+        <v>279</v>
       </c>
       <c r="H52" s="14" t="s">
-        <v>253</v>
+        <v>280</v>
       </c>
       <c r="I52" s="14" t="s">
-        <v>254</v>
+        <v>281</v>
       </c>
       <c r="J52" s="15" t="s">
         <v>52</v>
@@ -4267,16 +4342,16 @@
         <v>114</v>
       </c>
       <c r="F53" s="13" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="G53" s="14" t="s">
-        <v>255</v>
+        <v>282</v>
       </c>
       <c r="H53" s="14" t="s">
-        <v>256</v>
+        <v>283</v>
       </c>
       <c r="I53" s="14" t="s">
-        <v>257</v>
+        <v>284</v>
       </c>
       <c r="J53" s="15" t="s">
         <v>52</v>
@@ -4321,16 +4396,16 @@
         <v>116</v>
       </c>
       <c r="F54" s="13" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="G54" s="14" t="s">
-        <v>258</v>
+        <v>285</v>
       </c>
       <c r="H54" s="14" t="s">
-        <v>259</v>
+        <v>286</v>
       </c>
       <c r="I54" s="14" t="s">
-        <v>260</v>
+        <v>287</v>
       </c>
       <c r="J54" s="15" t="s">
         <v>52</v>
@@ -4375,16 +4450,16 @@
         <v>118</v>
       </c>
       <c r="F55" s="13" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="G55" s="14" t="s">
-        <v>261</v>
+        <v>288</v>
       </c>
       <c r="H55" s="14" t="s">
-        <v>262</v>
+        <v>289</v>
       </c>
       <c r="I55" s="14" t="s">
-        <v>263</v>
+        <v>290</v>
       </c>
       <c r="J55" s="15" t="s">
         <v>52</v>
@@ -4429,16 +4504,16 @@
         <v>120</v>
       </c>
       <c r="F56" s="13" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="G56" s="14" t="s">
-        <v>264</v>
+        <v>291</v>
       </c>
       <c r="H56" s="14" t="s">
-        <v>265</v>
+        <v>292</v>
       </c>
       <c r="I56" s="14" t="s">
-        <v>266</v>
+        <v>293</v>
       </c>
       <c r="J56" s="15" t="s">
         <v>52</v>
@@ -4483,16 +4558,16 @@
         <v>122</v>
       </c>
       <c r="F57" s="13" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="G57" s="14" t="s">
-        <v>267</v>
+        <v>294</v>
       </c>
       <c r="H57" s="14" t="s">
-        <v>268</v>
+        <v>295</v>
       </c>
       <c r="I57" s="14" t="s">
-        <v>269</v>
+        <v>296</v>
       </c>
       <c r="J57" s="15" t="s">
         <v>52</v>
@@ -4537,16 +4612,16 @@
         <v>124</v>
       </c>
       <c r="F58" s="13" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="G58" s="14" t="s">
-        <v>270</v>
+        <v>297</v>
       </c>
       <c r="H58" s="14" t="s">
-        <v>271</v>
+        <v>298</v>
       </c>
       <c r="I58" s="14" t="s">
-        <v>272</v>
+        <v>299</v>
       </c>
       <c r="J58" s="15" t="s">
         <v>52</v>
@@ -4591,16 +4666,16 @@
         <v>126</v>
       </c>
       <c r="F59" s="13" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="G59" s="14" t="s">
-        <v>273</v>
+        <v>300</v>
       </c>
       <c r="H59" s="14" t="s">
-        <v>274</v>
+        <v>301</v>
       </c>
       <c r="I59" s="14" t="s">
-        <v>275</v>
+        <v>302</v>
       </c>
       <c r="J59" s="15" t="s">
         <v>52</v>
@@ -4645,16 +4720,16 @@
         <v>128</v>
       </c>
       <c r="F60" s="13" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="G60" s="14" t="s">
-        <v>276</v>
+        <v>303</v>
       </c>
       <c r="H60" s="14" t="s">
-        <v>277</v>
+        <v>304</v>
       </c>
       <c r="I60" s="14" t="s">
-        <v>278</v>
+        <v>305</v>
       </c>
       <c r="J60" s="15" t="s">
         <v>52</v>

</xml_diff>

<commit_message>
Modifica Excel per Gestione Errore
Modifica file Excel per l'aggiunta dell'informazione Gestione Errore
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#150203000000XX/ASL_Caserta/ASLCE_ADTPS/1.0/report-checklist.xlsx
+++ b/GATEWAY/A1#150203000000XX/ASL_Caserta/ASLCE_ADTPS/1.0/report-checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dario.sommonte\Documents\DOCUMENTI UFFICIO\FSE-CDA2\AGGIORNAMENTO FSE2\ACCREDITAMENTO\GATEWAY\A1#150203000000XX\ASL_Caserta\ASLCE_ADTPS\1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E129392C-5AA6-41E9-9F16-952B7801A804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C89D405D-8733-4CB3-B412-41B3B8A07DE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="630" windowWidth="28770" windowHeight="15570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="3" r:id="rId1"/>
@@ -21,11 +21,6 @@
     <definedName name="filtro" localSheetId="0">TestCases!$A$9:$S$35</definedName>
   </definedNames>
   <calcPr calcId="0"/>
-  <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataSignature="AMtx7mhUlYP9yzNmk4f07XMJovPPUaqOhw=="/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -62,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="307">
   <si>
     <t>NOME FORNITORE:</t>
   </si>
@@ -723,9 +718,6 @@
     <t>Il software esegue automaticamente l'uppercase del campo CF</t>
   </si>
   <si>
-    <t>IL SERVIZIO MOSTRA UN MESSAGGIO DI ERRORE INTERNO E TENTA IL REINVIO</t>
-  </si>
-  <si>
     <t>Terapia farmacologica viene valorizzata come campo testuale</t>
   </si>
   <si>
@@ -1225,6 +1217,12 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.150.4.4.05749625b2397823fb6e622bd34c86f95d4204a8d88eda08af3467630d91b2bd.32b6742cb5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>Visualizzazione errore di connessione al servizio all'operatore.</t>
+  </si>
+  <si>
+    <t>Il servizio mostra un messaggio di errata compilazione del documento, l'utente dovrà correggerlo e procedere all'invio. Il sistema memorizza in una tabella di audit il log degli errori</t>
   </si>
 </sst>
 </file>
@@ -1481,7 +1479,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1570,6 +1568,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1866,10 +1870,10 @@
   <dimension ref="A1:T678"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="E52" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="F55" sqref="F55:I60"/>
+      <selection pane="bottomRight" activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2140,16 +2144,16 @@
         <v>28</v>
       </c>
       <c r="F10" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="G10" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="G10" s="14" t="s">
+      <c r="H10" s="14" t="s">
         <v>172</v>
       </c>
-      <c r="H10" s="14" t="s">
+      <c r="I10" s="14" t="s">
         <v>173</v>
-      </c>
-      <c r="I10" s="14" t="s">
-        <v>174</v>
       </c>
       <c r="J10" s="20" t="s">
         <v>52</v>
@@ -2158,12 +2162,8 @@
       <c r="L10" s="15"/>
       <c r="M10" s="15"/>
       <c r="N10" s="15"/>
-      <c r="O10" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="P10" s="15" t="s">
-        <v>52</v>
-      </c>
+      <c r="O10" s="15"/>
+      <c r="P10" s="15"/>
       <c r="Q10" s="15"/>
       <c r="R10" s="16"/>
       <c r="S10" s="17"/>
@@ -2188,16 +2188,16 @@
         <v>30</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G11" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="H11" s="14" t="s">
         <v>175</v>
       </c>
-      <c r="H11" s="14" t="s">
+      <c r="I11" s="14" t="s">
         <v>176</v>
-      </c>
-      <c r="I11" s="14" t="s">
-        <v>177</v>
       </c>
       <c r="J11" s="20" t="s">
         <v>52</v>
@@ -2206,12 +2206,8 @@
       <c r="L11" s="15"/>
       <c r="M11" s="15"/>
       <c r="N11" s="15"/>
-      <c r="O11" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="P11" s="15" t="s">
-        <v>52</v>
-      </c>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
       <c r="Q11" s="15"/>
       <c r="R11" s="16"/>
       <c r="S11" s="17"/>
@@ -2236,16 +2232,16 @@
         <v>32</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G12" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="H12" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="H12" s="14" t="s">
+      <c r="I12" s="14" t="s">
         <v>179</v>
-      </c>
-      <c r="I12" s="14" t="s">
-        <v>180</v>
       </c>
       <c r="J12" s="20" t="s">
         <v>52</v>
@@ -2254,12 +2250,8 @@
       <c r="L12" s="15"/>
       <c r="M12" s="15"/>
       <c r="N12" s="15"/>
-      <c r="O12" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="P12" s="15" t="s">
-        <v>52</v>
-      </c>
+      <c r="O12" s="15"/>
+      <c r="P12" s="15"/>
       <c r="Q12" s="15"/>
       <c r="R12" s="16"/>
       <c r="S12" s="17"/>
@@ -2284,16 +2276,16 @@
         <v>34</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G13" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="H13" s="14" t="s">
         <v>181</v>
       </c>
-      <c r="H13" s="14" t="s">
+      <c r="I13" s="14" t="s">
         <v>182</v>
-      </c>
-      <c r="I13" s="14" t="s">
-        <v>183</v>
       </c>
       <c r="J13" s="20" t="s">
         <v>52</v>
@@ -2302,12 +2294,8 @@
       <c r="L13" s="15"/>
       <c r="M13" s="15"/>
       <c r="N13" s="15"/>
-      <c r="O13" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="P13" s="15" t="s">
-        <v>52</v>
-      </c>
+      <c r="O13" s="15"/>
+      <c r="P13" s="15"/>
       <c r="Q13" s="15"/>
       <c r="R13" s="16"/>
       <c r="S13" s="17"/>
@@ -2332,16 +2320,16 @@
         <v>36</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G14" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="H14" s="14" t="s">
         <v>184</v>
       </c>
-      <c r="H14" s="14" t="s">
+      <c r="I14" s="14" t="s">
         <v>185</v>
-      </c>
-      <c r="I14" s="14" t="s">
-        <v>186</v>
       </c>
       <c r="J14" s="20" t="s">
         <v>52</v>
@@ -2350,12 +2338,8 @@
       <c r="L14" s="15"/>
       <c r="M14" s="15"/>
       <c r="N14" s="15"/>
-      <c r="O14" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="P14" s="15" t="s">
-        <v>52</v>
-      </c>
+      <c r="O14" s="15"/>
+      <c r="P14" s="15"/>
       <c r="Q14" s="15"/>
       <c r="R14" s="16"/>
       <c r="S14" s="17"/>
@@ -2380,16 +2364,16 @@
         <v>38</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G15" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="H15" s="14" t="s">
         <v>187</v>
       </c>
-      <c r="H15" s="14" t="s">
+      <c r="I15" s="14" t="s">
         <v>188</v>
-      </c>
-      <c r="I15" s="14" t="s">
-        <v>189</v>
       </c>
       <c r="J15" s="20" t="s">
         <v>52</v>
@@ -2398,12 +2382,8 @@
       <c r="L15" s="15"/>
       <c r="M15" s="15"/>
       <c r="N15" s="15"/>
-      <c r="O15" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="P15" s="15" t="s">
-        <v>52</v>
-      </c>
+      <c r="O15" s="15"/>
+      <c r="P15" s="15"/>
       <c r="Q15" s="15"/>
       <c r="R15" s="16"/>
       <c r="S15" s="17"/>
@@ -2428,16 +2408,16 @@
         <v>40</v>
       </c>
       <c r="F16" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G16" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="H16" s="14" t="s">
         <v>190</v>
       </c>
-      <c r="H16" s="14" t="s">
+      <c r="I16" s="14" t="s">
         <v>191</v>
-      </c>
-      <c r="I16" s="14" t="s">
-        <v>192</v>
       </c>
       <c r="J16" s="20" t="s">
         <v>52</v>
@@ -2446,12 +2426,8 @@
       <c r="L16" s="15"/>
       <c r="M16" s="15"/>
       <c r="N16" s="15"/>
-      <c r="O16" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="P16" s="15" t="s">
-        <v>52</v>
-      </c>
+      <c r="O16" s="15"/>
+      <c r="P16" s="15"/>
       <c r="Q16" s="15"/>
       <c r="R16" s="16"/>
       <c r="S16" s="17"/>
@@ -2476,16 +2452,16 @@
         <v>42</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G17" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="H17" s="14" t="s">
         <v>193</v>
       </c>
-      <c r="H17" s="14" t="s">
+      <c r="I17" s="14" t="s">
         <v>194</v>
-      </c>
-      <c r="I17" s="14" t="s">
-        <v>195</v>
       </c>
       <c r="J17" s="20" t="s">
         <v>52</v>
@@ -2494,12 +2470,8 @@
       <c r="L17" s="15"/>
       <c r="M17" s="15"/>
       <c r="N17" s="15"/>
-      <c r="O17" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="P17" s="15" t="s">
-        <v>52</v>
-      </c>
+      <c r="O17" s="15"/>
+      <c r="P17" s="15"/>
       <c r="Q17" s="15"/>
       <c r="R17" s="16"/>
       <c r="S17" s="17"/>
@@ -2524,13 +2496,13 @@
         <v>44</v>
       </c>
       <c r="F18" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G18" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="H18" s="14" t="s">
         <v>196</v>
-      </c>
-      <c r="H18" s="14" t="s">
-        <v>197</v>
       </c>
       <c r="I18" s="14" t="s">
         <v>136</v>
@@ -2546,18 +2518,16 @@
         <v>52</v>
       </c>
       <c r="N18" s="15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="O18" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="P18" s="15" t="s">
-        <v>52</v>
-      </c>
+      <c r="P18" s="15"/>
       <c r="Q18" s="15"/>
       <c r="R18" s="16"/>
       <c r="S18" s="22" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="T18" s="18" t="s">
         <v>23</v>
@@ -2580,13 +2550,13 @@
         <v>46</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G19" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="H19" s="14" t="s">
         <v>198</v>
-      </c>
-      <c r="H19" s="14" t="s">
-        <v>199</v>
       </c>
       <c r="I19" s="14" t="s">
         <v>136</v>
@@ -2602,18 +2572,16 @@
         <v>52</v>
       </c>
       <c r="N19" s="15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="O19" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="P19" s="15" t="s">
-        <v>52</v>
-      </c>
+      <c r="P19" s="15"/>
       <c r="Q19" s="15"/>
       <c r="R19" s="16"/>
       <c r="S19" s="22" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="T19" s="18" t="s">
         <v>23</v>
@@ -2636,13 +2604,13 @@
         <v>48</v>
       </c>
       <c r="F20" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G20" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="H20" s="14" t="s">
         <v>200</v>
-      </c>
-      <c r="H20" s="14" t="s">
-        <v>201</v>
       </c>
       <c r="I20" s="14" t="s">
         <v>136</v>
@@ -2658,18 +2626,16 @@
         <v>52</v>
       </c>
       <c r="N20" s="15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="O20" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="P20" s="15" t="s">
-        <v>52</v>
-      </c>
+      <c r="P20" s="15"/>
       <c r="Q20" s="15"/>
       <c r="R20" s="16"/>
       <c r="S20" s="22" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="T20" s="18" t="s">
         <v>23</v>
@@ -2692,13 +2658,13 @@
         <v>50</v>
       </c>
       <c r="F21" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G21" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="H21" s="14" t="s">
         <v>202</v>
-      </c>
-      <c r="H21" s="14" t="s">
-        <v>203</v>
       </c>
       <c r="I21" s="14" t="s">
         <v>136</v>
@@ -2714,18 +2680,16 @@
         <v>52</v>
       </c>
       <c r="N21" s="15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="O21" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="P21" s="15" t="s">
-        <v>52</v>
-      </c>
+      <c r="P21" s="15"/>
       <c r="Q21" s="15"/>
       <c r="R21" s="16"/>
       <c r="S21" s="22" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="T21" s="18" t="s">
         <v>23</v>
@@ -2757,8 +2721,8 @@
       <c r="M22" s="15"/>
       <c r="N22" s="15"/>
       <c r="O22" s="15"/>
-      <c r="P22" s="20" t="s">
-        <v>138</v>
+      <c r="P22" s="36" t="s">
+        <v>305</v>
       </c>
       <c r="Q22" s="20"/>
       <c r="R22" s="21" t="s">
@@ -2795,8 +2759,8 @@
       <c r="M23" s="15"/>
       <c r="N23" s="15"/>
       <c r="O23" s="15"/>
-      <c r="P23" s="20" t="s">
-        <v>138</v>
+      <c r="P23" s="37" t="s">
+        <v>305</v>
       </c>
       <c r="Q23" s="20"/>
       <c r="R23" s="21" t="s">
@@ -2824,16 +2788,16 @@
         <v>56</v>
       </c>
       <c r="F24" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G24" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="H24" s="14" t="s">
         <v>204</v>
       </c>
-      <c r="H24" s="14" t="s">
+      <c r="I24" s="14" t="s">
         <v>205</v>
-      </c>
-      <c r="I24" s="14" t="s">
-        <v>206</v>
       </c>
       <c r="J24" s="15" t="s">
         <v>52</v>
@@ -2846,13 +2810,13 @@
         <v>131</v>
       </c>
       <c r="N24" s="15" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="O24" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P24" s="15" t="s">
-        <v>52</v>
+      <c r="P24" s="37" t="s">
+        <v>306</v>
       </c>
       <c r="Q24" s="15"/>
       <c r="R24" s="16"/>
@@ -2916,16 +2880,16 @@
         <v>60</v>
       </c>
       <c r="F26" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G26" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="H26" s="14" t="s">
         <v>207</v>
       </c>
-      <c r="H26" s="14" t="s">
+      <c r="I26" s="14" t="s">
         <v>208</v>
-      </c>
-      <c r="I26" s="14" t="s">
-        <v>209</v>
       </c>
       <c r="J26" s="15" t="s">
         <v>52</v>
@@ -2938,13 +2902,13 @@
         <v>52</v>
       </c>
       <c r="N26" s="15" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="O26" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P26" s="15" t="s">
-        <v>52</v>
+      <c r="P26" s="37" t="s">
+        <v>306</v>
       </c>
       <c r="Q26" s="15"/>
       <c r="R26" s="16"/>
@@ -2970,16 +2934,16 @@
         <v>62</v>
       </c>
       <c r="F27" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G27" s="14" t="s">
+        <v>209</v>
+      </c>
+      <c r="H27" s="14" t="s">
         <v>210</v>
       </c>
-      <c r="H27" s="14" t="s">
+      <c r="I27" s="14" t="s">
         <v>211</v>
-      </c>
-      <c r="I27" s="14" t="s">
-        <v>212</v>
       </c>
       <c r="J27" s="15" t="s">
         <v>52</v>
@@ -2992,13 +2956,13 @@
         <v>52</v>
       </c>
       <c r="N27" s="15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="O27" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P27" s="15" t="s">
-        <v>52</v>
+      <c r="P27" s="37" t="s">
+        <v>306</v>
       </c>
       <c r="Q27" s="15"/>
       <c r="R27" s="16"/>
@@ -3024,16 +2988,16 @@
         <v>64</v>
       </c>
       <c r="F28" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G28" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="H28" s="14" t="s">
         <v>213</v>
       </c>
-      <c r="H28" s="14" t="s">
+      <c r="I28" s="14" t="s">
         <v>214</v>
-      </c>
-      <c r="I28" s="14" t="s">
-        <v>215</v>
       </c>
       <c r="J28" s="15" t="s">
         <v>52</v>
@@ -3046,13 +3010,13 @@
         <v>52</v>
       </c>
       <c r="N28" s="15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="O28" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P28" s="15" t="s">
-        <v>52</v>
+      <c r="P28" s="37" t="s">
+        <v>306</v>
       </c>
       <c r="Q28" s="15"/>
       <c r="R28" s="16"/>
@@ -3078,16 +3042,16 @@
         <v>66</v>
       </c>
       <c r="F29" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G29" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="H29" s="14" t="s">
         <v>216</v>
       </c>
-      <c r="H29" s="14" t="s">
+      <c r="I29" s="14" t="s">
         <v>217</v>
-      </c>
-      <c r="I29" s="14" t="s">
-        <v>218</v>
       </c>
       <c r="J29" s="15" t="s">
         <v>52</v>
@@ -3100,13 +3064,13 @@
         <v>52</v>
       </c>
       <c r="N29" s="15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="O29" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P29" s="15" t="s">
-        <v>52</v>
+      <c r="P29" s="37" t="s">
+        <v>306</v>
       </c>
       <c r="Q29" s="15"/>
       <c r="R29" s="16"/>
@@ -3132,16 +3096,16 @@
         <v>68</v>
       </c>
       <c r="F30" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G30" s="14" t="s">
+        <v>218</v>
+      </c>
+      <c r="H30" s="14" t="s">
         <v>219</v>
       </c>
-      <c r="H30" s="14" t="s">
+      <c r="I30" s="14" t="s">
         <v>220</v>
-      </c>
-      <c r="I30" s="14" t="s">
-        <v>221</v>
       </c>
       <c r="J30" s="15" t="s">
         <v>52</v>
@@ -3154,13 +3118,13 @@
         <v>52</v>
       </c>
       <c r="N30" s="15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="O30" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P30" s="15" t="s">
-        <v>52</v>
+      <c r="P30" s="37" t="s">
+        <v>306</v>
       </c>
       <c r="Q30" s="15"/>
       <c r="R30" s="16"/>
@@ -3186,16 +3150,16 @@
         <v>70</v>
       </c>
       <c r="F31" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G31" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="H31" s="14" t="s">
         <v>222</v>
       </c>
-      <c r="H31" s="14" t="s">
+      <c r="I31" s="14" t="s">
         <v>223</v>
-      </c>
-      <c r="I31" s="14" t="s">
-        <v>224</v>
       </c>
       <c r="J31" s="15" t="s">
         <v>52</v>
@@ -3208,13 +3172,13 @@
         <v>52</v>
       </c>
       <c r="N31" s="15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="O31" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P31" s="15" t="s">
-        <v>52</v>
+      <c r="P31" s="37" t="s">
+        <v>306</v>
       </c>
       <c r="Q31" s="15"/>
       <c r="R31" s="16"/>
@@ -3240,16 +3204,16 @@
         <v>72</v>
       </c>
       <c r="F32" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G32" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="H32" s="14" t="s">
         <v>225</v>
       </c>
-      <c r="H32" s="14" t="s">
+      <c r="I32" s="14" t="s">
         <v>226</v>
-      </c>
-      <c r="I32" s="14" t="s">
-        <v>227</v>
       </c>
       <c r="J32" s="15" t="s">
         <v>52</v>
@@ -3262,13 +3226,13 @@
         <v>52</v>
       </c>
       <c r="N32" s="15" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="O32" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P32" s="15" t="s">
-        <v>52</v>
+      <c r="P32" s="37" t="s">
+        <v>306</v>
       </c>
       <c r="Q32" s="15"/>
       <c r="R32" s="16"/>
@@ -3294,16 +3258,16 @@
         <v>74</v>
       </c>
       <c r="F33" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G33" s="14" t="s">
+        <v>227</v>
+      </c>
+      <c r="H33" s="14" t="s">
         <v>228</v>
       </c>
-      <c r="H33" s="14" t="s">
+      <c r="I33" s="14" t="s">
         <v>229</v>
-      </c>
-      <c r="I33" s="14" t="s">
-        <v>230</v>
       </c>
       <c r="J33" s="15" t="s">
         <v>52</v>
@@ -3316,13 +3280,13 @@
         <v>52</v>
       </c>
       <c r="N33" s="15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O33" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P33" s="15" t="s">
-        <v>52</v>
+      <c r="P33" s="37" t="s">
+        <v>306</v>
       </c>
       <c r="Q33" s="15"/>
       <c r="R33" s="16"/>
@@ -3348,16 +3312,16 @@
         <v>76</v>
       </c>
       <c r="F34" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G34" s="14" t="s">
+        <v>230</v>
+      </c>
+      <c r="H34" s="14" t="s">
         <v>231</v>
       </c>
-      <c r="H34" s="14" t="s">
+      <c r="I34" s="14" t="s">
         <v>232</v>
-      </c>
-      <c r="I34" s="14" t="s">
-        <v>233</v>
       </c>
       <c r="J34" s="15" t="s">
         <v>52</v>
@@ -3370,13 +3334,13 @@
         <v>52</v>
       </c>
       <c r="N34" s="15" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="O34" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P34" s="15" t="s">
-        <v>52</v>
+      <c r="P34" s="37" t="s">
+        <v>306</v>
       </c>
       <c r="Q34" s="15"/>
       <c r="R34" s="16"/>
@@ -3409,7 +3373,7 @@
         <v>131</v>
       </c>
       <c r="K35" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L35" s="15"/>
       <c r="M35" s="15"/>
@@ -3423,7 +3387,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="19">
         <v>122</v>
       </c>
@@ -3440,16 +3404,16 @@
         <v>80</v>
       </c>
       <c r="F36" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G36" s="14" t="s">
+        <v>233</v>
+      </c>
+      <c r="H36" s="14" t="s">
         <v>234</v>
       </c>
-      <c r="H36" s="14" t="s">
+      <c r="I36" s="14" t="s">
         <v>235</v>
-      </c>
-      <c r="I36" s="14" t="s">
-        <v>236</v>
       </c>
       <c r="J36" s="15" t="s">
         <v>52</v>
@@ -3462,13 +3426,13 @@
         <v>131</v>
       </c>
       <c r="N36" s="15" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="O36" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P36" s="15" t="s">
-        <v>52</v>
+      <c r="P36" s="37" t="s">
+        <v>306</v>
       </c>
       <c r="Q36" s="15"/>
       <c r="R36" s="16"/>
@@ -3515,7 +3479,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="19">
         <v>124</v>
       </c>
@@ -3532,16 +3496,16 @@
         <v>84</v>
       </c>
       <c r="F38" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G38" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="H38" s="14" t="s">
         <v>237</v>
       </c>
-      <c r="H38" s="14" t="s">
+      <c r="I38" s="14" t="s">
         <v>238</v>
-      </c>
-      <c r="I38" s="14" t="s">
-        <v>239</v>
       </c>
       <c r="J38" s="15" t="s">
         <v>52</v>
@@ -3554,13 +3518,13 @@
         <v>52</v>
       </c>
       <c r="N38" s="15" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="O38" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P38" s="15" t="s">
-        <v>52</v>
+      <c r="P38" s="37" t="s">
+        <v>306</v>
       </c>
       <c r="Q38" s="15"/>
       <c r="R38" s="16"/>
@@ -3586,16 +3550,16 @@
         <v>86</v>
       </c>
       <c r="F39" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G39" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="H39" s="14" t="s">
         <v>240</v>
       </c>
-      <c r="H39" s="14" t="s">
+      <c r="I39" s="14" t="s">
         <v>241</v>
-      </c>
-      <c r="I39" s="14" t="s">
-        <v>242</v>
       </c>
       <c r="J39" s="15" t="s">
         <v>52</v>
@@ -3608,13 +3572,13 @@
         <v>52</v>
       </c>
       <c r="N39" s="15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="O39" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P39" s="15" t="s">
-        <v>52</v>
+      <c r="P39" s="37" t="s">
+        <v>306</v>
       </c>
       <c r="Q39" s="15"/>
       <c r="R39" s="16"/>
@@ -3623,7 +3587,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="19">
         <v>126</v>
       </c>
@@ -3640,16 +3604,16 @@
         <v>88</v>
       </c>
       <c r="F40" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G40" s="14" t="s">
+        <v>242</v>
+      </c>
+      <c r="H40" s="14" t="s">
         <v>243</v>
       </c>
-      <c r="H40" s="14" t="s">
+      <c r="I40" s="14" t="s">
         <v>244</v>
-      </c>
-      <c r="I40" s="14" t="s">
-        <v>245</v>
       </c>
       <c r="J40" s="15" t="s">
         <v>52</v>
@@ -3662,13 +3626,13 @@
         <v>52</v>
       </c>
       <c r="N40" s="15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="O40" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P40" s="15" t="s">
-        <v>52</v>
+      <c r="P40" s="37" t="s">
+        <v>306</v>
       </c>
       <c r="Q40" s="15"/>
       <c r="R40" s="16"/>
@@ -3694,16 +3658,16 @@
         <v>90</v>
       </c>
       <c r="F41" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G41" s="14" t="s">
+        <v>245</v>
+      </c>
+      <c r="H41" s="14" t="s">
         <v>246</v>
       </c>
-      <c r="H41" s="14" t="s">
+      <c r="I41" s="14" t="s">
         <v>247</v>
-      </c>
-      <c r="I41" s="14" t="s">
-        <v>248</v>
       </c>
       <c r="J41" s="15" t="s">
         <v>52</v>
@@ -3716,13 +3680,13 @@
         <v>52</v>
       </c>
       <c r="N41" s="15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="O41" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P41" s="15" t="s">
-        <v>52</v>
+      <c r="P41" s="37" t="s">
+        <v>306</v>
       </c>
       <c r="Q41" s="15"/>
       <c r="R41" s="16"/>
@@ -3748,16 +3712,16 @@
         <v>92</v>
       </c>
       <c r="F42" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G42" s="14" t="s">
+        <v>248</v>
+      </c>
+      <c r="H42" s="14" t="s">
         <v>249</v>
       </c>
-      <c r="H42" s="14" t="s">
+      <c r="I42" s="14" t="s">
         <v>250</v>
-      </c>
-      <c r="I42" s="14" t="s">
-        <v>251</v>
       </c>
       <c r="J42" s="15" t="s">
         <v>52</v>
@@ -3770,13 +3734,13 @@
         <v>52</v>
       </c>
       <c r="N42" s="15" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="O42" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P42" s="15" t="s">
-        <v>52</v>
+      <c r="P42" s="37" t="s">
+        <v>306</v>
       </c>
       <c r="Q42" s="15"/>
       <c r="R42" s="16"/>
@@ -3802,16 +3766,16 @@
         <v>94</v>
       </c>
       <c r="F43" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G43" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="H43" s="14" t="s">
         <v>252</v>
       </c>
-      <c r="H43" s="14" t="s">
+      <c r="I43" s="14" t="s">
         <v>253</v>
-      </c>
-      <c r="I43" s="14" t="s">
-        <v>254</v>
       </c>
       <c r="J43" s="15" t="s">
         <v>52</v>
@@ -3824,13 +3788,13 @@
         <v>52</v>
       </c>
       <c r="N43" s="15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="O43" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P43" s="15" t="s">
-        <v>52</v>
+      <c r="P43" s="37" t="s">
+        <v>306</v>
       </c>
       <c r="Q43" s="15"/>
       <c r="R43" s="16"/>
@@ -3856,16 +3820,16 @@
         <v>96</v>
       </c>
       <c r="F44" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G44" s="14" t="s">
+        <v>254</v>
+      </c>
+      <c r="H44" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="H44" s="14" t="s">
+      <c r="I44" s="14" t="s">
         <v>256</v>
-      </c>
-      <c r="I44" s="14" t="s">
-        <v>257</v>
       </c>
       <c r="J44" s="15" t="s">
         <v>52</v>
@@ -3878,13 +3842,13 @@
         <v>52</v>
       </c>
       <c r="N44" s="15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="O44" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P44" s="15" t="s">
-        <v>52</v>
+      <c r="P44" s="37" t="s">
+        <v>306</v>
       </c>
       <c r="Q44" s="15"/>
       <c r="R44" s="16"/>
@@ -3910,16 +3874,16 @@
         <v>98</v>
       </c>
       <c r="F45" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G45" s="14" t="s">
+        <v>257</v>
+      </c>
+      <c r="H45" s="14" t="s">
         <v>258</v>
       </c>
-      <c r="H45" s="14" t="s">
+      <c r="I45" s="14" t="s">
         <v>259</v>
-      </c>
-      <c r="I45" s="14" t="s">
-        <v>260</v>
       </c>
       <c r="J45" s="15" t="s">
         <v>52</v>
@@ -3932,13 +3896,13 @@
         <v>52</v>
       </c>
       <c r="N45" s="15" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="O45" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P45" s="15" t="s">
-        <v>52</v>
+      <c r="P45" s="37" t="s">
+        <v>306</v>
       </c>
       <c r="Q45" s="15"/>
       <c r="R45" s="16"/>
@@ -3964,16 +3928,16 @@
         <v>100</v>
       </c>
       <c r="F46" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G46" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="H46" s="14" t="s">
         <v>261</v>
       </c>
-      <c r="H46" s="14" t="s">
+      <c r="I46" s="14" t="s">
         <v>262</v>
-      </c>
-      <c r="I46" s="14" t="s">
-        <v>263</v>
       </c>
       <c r="J46" s="15" t="s">
         <v>52</v>
@@ -3986,13 +3950,13 @@
         <v>52</v>
       </c>
       <c r="N46" s="15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="O46" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P46" s="15" t="s">
-        <v>52</v>
+      <c r="P46" s="37" t="s">
+        <v>306</v>
       </c>
       <c r="Q46" s="15"/>
       <c r="R46" s="16"/>
@@ -4018,16 +3982,16 @@
         <v>102</v>
       </c>
       <c r="F47" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G47" s="14" t="s">
+        <v>263</v>
+      </c>
+      <c r="H47" s="14" t="s">
         <v>264</v>
       </c>
-      <c r="H47" s="14" t="s">
+      <c r="I47" s="14" t="s">
         <v>265</v>
-      </c>
-      <c r="I47" s="14" t="s">
-        <v>266</v>
       </c>
       <c r="J47" s="15" t="s">
         <v>52</v>
@@ -4040,13 +4004,13 @@
         <v>52</v>
       </c>
       <c r="N47" s="15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O47" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P47" s="15" t="s">
-        <v>52</v>
+      <c r="P47" s="37" t="s">
+        <v>306</v>
       </c>
       <c r="Q47" s="15"/>
       <c r="R47" s="16"/>
@@ -4072,16 +4036,16 @@
         <v>104</v>
       </c>
       <c r="F48" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G48" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="H48" s="14" t="s">
         <v>267</v>
       </c>
-      <c r="H48" s="14" t="s">
+      <c r="I48" s="14" t="s">
         <v>268</v>
-      </c>
-      <c r="I48" s="14" t="s">
-        <v>269</v>
       </c>
       <c r="J48" s="15" t="s">
         <v>52</v>
@@ -4094,13 +4058,13 @@
         <v>52</v>
       </c>
       <c r="N48" s="15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="O48" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P48" s="15" t="s">
-        <v>52</v>
+      <c r="P48" s="37" t="s">
+        <v>306</v>
       </c>
       <c r="Q48" s="15"/>
       <c r="R48" s="16"/>
@@ -4126,16 +4090,16 @@
         <v>106</v>
       </c>
       <c r="F49" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G49" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="H49" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="H49" s="14" t="s">
+      <c r="I49" s="14" t="s">
         <v>271</v>
-      </c>
-      <c r="I49" s="14" t="s">
-        <v>272</v>
       </c>
       <c r="J49" s="15" t="s">
         <v>52</v>
@@ -4148,13 +4112,13 @@
         <v>52</v>
       </c>
       <c r="N49" s="15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="O49" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P49" s="15" t="s">
-        <v>52</v>
+      <c r="P49" s="37" t="s">
+        <v>306</v>
       </c>
       <c r="Q49" s="15"/>
       <c r="R49" s="16"/>
@@ -4180,16 +4144,16 @@
         <v>108</v>
       </c>
       <c r="F50" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G50" s="14" t="s">
+        <v>272</v>
+      </c>
+      <c r="H50" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="H50" s="14" t="s">
+      <c r="I50" s="14" t="s">
         <v>274</v>
-      </c>
-      <c r="I50" s="14" t="s">
-        <v>275</v>
       </c>
       <c r="J50" s="15" t="s">
         <v>52</v>
@@ -4202,13 +4166,13 @@
         <v>52</v>
       </c>
       <c r="N50" s="15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="O50" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P50" s="15" t="s">
-        <v>52</v>
+      <c r="P50" s="37" t="s">
+        <v>306</v>
       </c>
       <c r="Q50" s="15"/>
       <c r="R50" s="16"/>
@@ -4234,16 +4198,16 @@
         <v>110</v>
       </c>
       <c r="F51" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G51" s="14" t="s">
+        <v>275</v>
+      </c>
+      <c r="H51" s="14" t="s">
         <v>276</v>
       </c>
-      <c r="H51" s="14" t="s">
+      <c r="I51" s="14" t="s">
         <v>277</v>
-      </c>
-      <c r="I51" s="14" t="s">
-        <v>278</v>
       </c>
       <c r="J51" s="15" t="s">
         <v>52</v>
@@ -4256,13 +4220,13 @@
         <v>52</v>
       </c>
       <c r="N51" s="15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="O51" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P51" s="15" t="s">
-        <v>52</v>
+      <c r="P51" s="37" t="s">
+        <v>306</v>
       </c>
       <c r="Q51" s="15"/>
       <c r="R51" s="16"/>
@@ -4288,16 +4252,16 @@
         <v>112</v>
       </c>
       <c r="F52" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G52" s="14" t="s">
+        <v>278</v>
+      </c>
+      <c r="H52" s="14" t="s">
         <v>279</v>
       </c>
-      <c r="H52" s="14" t="s">
+      <c r="I52" s="14" t="s">
         <v>280</v>
-      </c>
-      <c r="I52" s="14" t="s">
-        <v>281</v>
       </c>
       <c r="J52" s="15" t="s">
         <v>52</v>
@@ -4310,13 +4274,13 @@
         <v>52</v>
       </c>
       <c r="N52" s="15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="O52" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P52" s="15" t="s">
-        <v>52</v>
+      <c r="P52" s="37" t="s">
+        <v>306</v>
       </c>
       <c r="Q52" s="15"/>
       <c r="R52" s="16"/>
@@ -4342,16 +4306,16 @@
         <v>114</v>
       </c>
       <c r="F53" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G53" s="14" t="s">
+        <v>281</v>
+      </c>
+      <c r="H53" s="14" t="s">
         <v>282</v>
       </c>
-      <c r="H53" s="14" t="s">
+      <c r="I53" s="14" t="s">
         <v>283</v>
-      </c>
-      <c r="I53" s="14" t="s">
-        <v>284</v>
       </c>
       <c r="J53" s="15" t="s">
         <v>52</v>
@@ -4364,13 +4328,13 @@
         <v>52</v>
       </c>
       <c r="N53" s="15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O53" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P53" s="15" t="s">
-        <v>52</v>
+      <c r="P53" s="37" t="s">
+        <v>306</v>
       </c>
       <c r="Q53" s="15"/>
       <c r="R53" s="16"/>
@@ -4396,16 +4360,16 @@
         <v>116</v>
       </c>
       <c r="F54" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G54" s="14" t="s">
+        <v>284</v>
+      </c>
+      <c r="H54" s="14" t="s">
         <v>285</v>
       </c>
-      <c r="H54" s="14" t="s">
+      <c r="I54" s="14" t="s">
         <v>286</v>
-      </c>
-      <c r="I54" s="14" t="s">
-        <v>287</v>
       </c>
       <c r="J54" s="15" t="s">
         <v>52</v>
@@ -4418,13 +4382,13 @@
         <v>52</v>
       </c>
       <c r="N54" s="15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="O54" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P54" s="15" t="s">
-        <v>52</v>
+      <c r="P54" s="37" t="s">
+        <v>306</v>
       </c>
       <c r="Q54" s="15"/>
       <c r="R54" s="16"/>
@@ -4450,16 +4414,16 @@
         <v>118</v>
       </c>
       <c r="F55" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G55" s="14" t="s">
+        <v>287</v>
+      </c>
+      <c r="H55" s="14" t="s">
         <v>288</v>
       </c>
-      <c r="H55" s="14" t="s">
+      <c r="I55" s="14" t="s">
         <v>289</v>
-      </c>
-      <c r="I55" s="14" t="s">
-        <v>290</v>
       </c>
       <c r="J55" s="15" t="s">
         <v>52</v>
@@ -4472,13 +4436,13 @@
         <v>52</v>
       </c>
       <c r="N55" s="15" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="O55" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P55" s="15" t="s">
-        <v>52</v>
+      <c r="P55" s="37" t="s">
+        <v>306</v>
       </c>
       <c r="Q55" s="15"/>
       <c r="R55" s="16"/>
@@ -4504,16 +4468,16 @@
         <v>120</v>
       </c>
       <c r="F56" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G56" s="14" t="s">
+        <v>290</v>
+      </c>
+      <c r="H56" s="14" t="s">
         <v>291</v>
       </c>
-      <c r="H56" s="14" t="s">
+      <c r="I56" s="14" t="s">
         <v>292</v>
-      </c>
-      <c r="I56" s="14" t="s">
-        <v>293</v>
       </c>
       <c r="J56" s="15" t="s">
         <v>52</v>
@@ -4526,13 +4490,13 @@
         <v>52</v>
       </c>
       <c r="N56" s="15" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="O56" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P56" s="15" t="s">
-        <v>52</v>
+      <c r="P56" s="37" t="s">
+        <v>306</v>
       </c>
       <c r="Q56" s="15"/>
       <c r="R56" s="16"/>
@@ -4558,16 +4522,16 @@
         <v>122</v>
       </c>
       <c r="F57" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G57" s="14" t="s">
+        <v>293</v>
+      </c>
+      <c r="H57" s="14" t="s">
         <v>294</v>
       </c>
-      <c r="H57" s="14" t="s">
+      <c r="I57" s="14" t="s">
         <v>295</v>
-      </c>
-      <c r="I57" s="14" t="s">
-        <v>296</v>
       </c>
       <c r="J57" s="15" t="s">
         <v>52</v>
@@ -4580,13 +4544,13 @@
         <v>52</v>
       </c>
       <c r="N57" s="15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="O57" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P57" s="15" t="s">
-        <v>52</v>
+      <c r="P57" s="37" t="s">
+        <v>306</v>
       </c>
       <c r="Q57" s="15"/>
       <c r="R57" s="16"/>
@@ -4612,16 +4576,16 @@
         <v>124</v>
       </c>
       <c r="F58" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G58" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="H58" s="14" t="s">
         <v>297</v>
       </c>
-      <c r="H58" s="14" t="s">
+      <c r="I58" s="14" t="s">
         <v>298</v>
-      </c>
-      <c r="I58" s="14" t="s">
-        <v>299</v>
       </c>
       <c r="J58" s="15" t="s">
         <v>52</v>
@@ -4634,13 +4598,13 @@
         <v>52</v>
       </c>
       <c r="N58" s="15" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="O58" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P58" s="15" t="s">
-        <v>52</v>
+      <c r="P58" s="37" t="s">
+        <v>306</v>
       </c>
       <c r="Q58" s="15"/>
       <c r="R58" s="16"/>
@@ -4666,16 +4630,16 @@
         <v>126</v>
       </c>
       <c r="F59" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G59" s="14" t="s">
+        <v>299</v>
+      </c>
+      <c r="H59" s="14" t="s">
         <v>300</v>
       </c>
-      <c r="H59" s="14" t="s">
+      <c r="I59" s="14" t="s">
         <v>301</v>
-      </c>
-      <c r="I59" s="14" t="s">
-        <v>302</v>
       </c>
       <c r="J59" s="15" t="s">
         <v>52</v>
@@ -4688,13 +4652,13 @@
         <v>52</v>
       </c>
       <c r="N59" s="15" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="O59" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P59" s="15" t="s">
-        <v>52</v>
+      <c r="P59" s="37" t="s">
+        <v>306</v>
       </c>
       <c r="Q59" s="15"/>
       <c r="R59" s="16"/>
@@ -4720,16 +4684,16 @@
         <v>128</v>
       </c>
       <c r="F60" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G60" s="14" t="s">
+        <v>302</v>
+      </c>
+      <c r="H60" s="14" t="s">
         <v>303</v>
       </c>
-      <c r="H60" s="14" t="s">
+      <c r="I60" s="14" t="s">
         <v>304</v>
-      </c>
-      <c r="I60" s="14" t="s">
-        <v>305</v>
       </c>
       <c r="J60" s="15" t="s">
         <v>52</v>
@@ -4742,13 +4706,13 @@
         <v>52</v>
       </c>
       <c r="N60" s="15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="O60" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P60" s="15" t="s">
-        <v>52</v>
+      <c r="P60" s="37" t="s">
+        <v>306</v>
       </c>
       <c r="Q60" s="15"/>
       <c r="R60" s="16"/>

</xml_diff>

<commit_message>
Aggiornamento Excel di accompagnamento
Aggiornamento Excel di accompagnamento per la compilazione della colonna Gestione errore anche per i casi gestiti in backoffice
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#150203000000XX/ASL_Caserta/ASLCE_ADTPS/1.0/report-checklist.xlsx
+++ b/GATEWAY/A1#150203000000XX/ASL_Caserta/ASLCE_ADTPS/1.0/report-checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dario.sommonte\Documents\DOCUMENTI UFFICIO\FSE-CDA2\AGGIORNAMENTO FSE2\ACCREDITAMENTO\GATEWAY\A1#150203000000XX\ASL_Caserta\ASLCE_ADTPS\1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C89D405D-8733-4CB3-B412-41B3B8A07DE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{042F2F62-AA7B-4CCF-9890-78D52147A2EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="3" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="308">
   <si>
     <t>NOME FORNITORE:</t>
   </si>
@@ -1219,10 +1219,13 @@
     <t>2.16.840.1.113883.2.9.2.150.4.4.05749625b2397823fb6e622bd34c86f95d4204a8d88eda08af3467630d91b2bd.32b6742cb5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>Visualizzazione errore di connessione al servizio all'operatore.</t>
-  </si>
-  <si>
     <t>Il servizio mostra un messaggio di errata compilazione del documento, l'utente dovrà correggerlo e procedere all'invio. Il sistema memorizza in una tabella di audit il log degli errori</t>
+  </si>
+  <si>
+    <t>L’errore si può verificare solo in caso di cambio di specifiche di generazione di token. Il sistema memorizza in una tabella di audit il log degli errori che viene gestito in back office dall'operatore informatico</t>
+  </si>
+  <si>
+    <t>Visualizzazione errore di connessione al servizio all'operatore sanitario che viene invitato a riprovare in seguito. L'operatore sanitario può ritentare l'invio del documento contestualmente o in modo massivo in una seconda fase.  Il sistema memorizza in una tabella di audit il log degli errori che viene monitorata dagli operatori informatici.</t>
   </si>
 </sst>
 </file>
@@ -1479,7 +1482,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1568,12 +1571,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1870,10 +1867,10 @@
   <dimension ref="A1:T678"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="E52" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="K32" sqref="K32"/>
+      <selection pane="bottomRight" activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2523,7 +2520,9 @@
       <c r="O18" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="P18" s="15"/>
+      <c r="P18" s="15" t="s">
+        <v>306</v>
+      </c>
       <c r="Q18" s="15"/>
       <c r="R18" s="16"/>
       <c r="S18" s="22" t="s">
@@ -2577,7 +2576,9 @@
       <c r="O19" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="P19" s="15"/>
+      <c r="P19" s="15" t="s">
+        <v>306</v>
+      </c>
       <c r="Q19" s="15"/>
       <c r="R19" s="16"/>
       <c r="S19" s="22" t="s">
@@ -2631,7 +2632,9 @@
       <c r="O20" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="P20" s="15"/>
+      <c r="P20" s="15" t="s">
+        <v>306</v>
+      </c>
       <c r="Q20" s="15"/>
       <c r="R20" s="16"/>
       <c r="S20" s="22" t="s">
@@ -2685,7 +2688,9 @@
       <c r="O21" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="P21" s="15"/>
+      <c r="P21" s="15" t="s">
+        <v>306</v>
+      </c>
       <c r="Q21" s="15"/>
       <c r="R21" s="16"/>
       <c r="S21" s="22" t="s">
@@ -2695,7 +2700,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="19">
         <v>45</v>
       </c>
@@ -2721,8 +2726,8 @@
       <c r="M22" s="15"/>
       <c r="N22" s="15"/>
       <c r="O22" s="15"/>
-      <c r="P22" s="36" t="s">
-        <v>305</v>
+      <c r="P22" s="15" t="s">
+        <v>307</v>
       </c>
       <c r="Q22" s="20"/>
       <c r="R22" s="21" t="s">
@@ -2733,7 +2738,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="19">
         <v>51</v>
       </c>
@@ -2759,8 +2764,8 @@
       <c r="M23" s="15"/>
       <c r="N23" s="15"/>
       <c r="O23" s="15"/>
-      <c r="P23" s="37" t="s">
-        <v>305</v>
+      <c r="P23" s="15" t="s">
+        <v>307</v>
       </c>
       <c r="Q23" s="20"/>
       <c r="R23" s="21" t="s">
@@ -2815,8 +2820,8 @@
       <c r="O24" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P24" s="37" t="s">
-        <v>306</v>
+      <c r="P24" s="15" t="s">
+        <v>305</v>
       </c>
       <c r="Q24" s="15"/>
       <c r="R24" s="16"/>
@@ -2907,8 +2912,8 @@
       <c r="O26" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P26" s="37" t="s">
-        <v>306</v>
+      <c r="P26" s="15" t="s">
+        <v>305</v>
       </c>
       <c r="Q26" s="15"/>
       <c r="R26" s="16"/>
@@ -2961,8 +2966,8 @@
       <c r="O27" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P27" s="37" t="s">
-        <v>306</v>
+      <c r="P27" s="15" t="s">
+        <v>305</v>
       </c>
       <c r="Q27" s="15"/>
       <c r="R27" s="16"/>
@@ -3015,8 +3020,8 @@
       <c r="O28" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P28" s="37" t="s">
-        <v>306</v>
+      <c r="P28" s="15" t="s">
+        <v>305</v>
       </c>
       <c r="Q28" s="15"/>
       <c r="R28" s="16"/>
@@ -3069,8 +3074,8 @@
       <c r="O29" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P29" s="37" t="s">
-        <v>306</v>
+      <c r="P29" s="15" t="s">
+        <v>305</v>
       </c>
       <c r="Q29" s="15"/>
       <c r="R29" s="16"/>
@@ -3123,8 +3128,8 @@
       <c r="O30" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P30" s="37" t="s">
-        <v>306</v>
+      <c r="P30" s="15" t="s">
+        <v>305</v>
       </c>
       <c r="Q30" s="15"/>
       <c r="R30" s="16"/>
@@ -3177,8 +3182,8 @@
       <c r="O31" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P31" s="37" t="s">
-        <v>306</v>
+      <c r="P31" s="15" t="s">
+        <v>305</v>
       </c>
       <c r="Q31" s="15"/>
       <c r="R31" s="16"/>
@@ -3231,8 +3236,8 @@
       <c r="O32" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P32" s="37" t="s">
-        <v>306</v>
+      <c r="P32" s="15" t="s">
+        <v>305</v>
       </c>
       <c r="Q32" s="15"/>
       <c r="R32" s="16"/>
@@ -3285,8 +3290,8 @@
       <c r="O33" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P33" s="37" t="s">
-        <v>306</v>
+      <c r="P33" s="15" t="s">
+        <v>305</v>
       </c>
       <c r="Q33" s="15"/>
       <c r="R33" s="16"/>
@@ -3339,8 +3344,8 @@
       <c r="O34" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P34" s="37" t="s">
-        <v>306</v>
+      <c r="P34" s="15" t="s">
+        <v>305</v>
       </c>
       <c r="Q34" s="15"/>
       <c r="R34" s="16"/>
@@ -3431,8 +3436,8 @@
       <c r="O36" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P36" s="37" t="s">
-        <v>306</v>
+      <c r="P36" s="15" t="s">
+        <v>305</v>
       </c>
       <c r="Q36" s="15"/>
       <c r="R36" s="16"/>
@@ -3523,8 +3528,8 @@
       <c r="O38" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P38" s="37" t="s">
-        <v>306</v>
+      <c r="P38" s="15" t="s">
+        <v>305</v>
       </c>
       <c r="Q38" s="15"/>
       <c r="R38" s="16"/>
@@ -3577,8 +3582,8 @@
       <c r="O39" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P39" s="37" t="s">
-        <v>306</v>
+      <c r="P39" s="15" t="s">
+        <v>305</v>
       </c>
       <c r="Q39" s="15"/>
       <c r="R39" s="16"/>
@@ -3631,8 +3636,8 @@
       <c r="O40" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P40" s="37" t="s">
-        <v>306</v>
+      <c r="P40" s="15" t="s">
+        <v>305</v>
       </c>
       <c r="Q40" s="15"/>
       <c r="R40" s="16"/>
@@ -3685,8 +3690,8 @@
       <c r="O41" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P41" s="37" t="s">
-        <v>306</v>
+      <c r="P41" s="15" t="s">
+        <v>305</v>
       </c>
       <c r="Q41" s="15"/>
       <c r="R41" s="16"/>
@@ -3739,8 +3744,8 @@
       <c r="O42" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P42" s="37" t="s">
-        <v>306</v>
+      <c r="P42" s="15" t="s">
+        <v>305</v>
       </c>
       <c r="Q42" s="15"/>
       <c r="R42" s="16"/>
@@ -3793,8 +3798,8 @@
       <c r="O43" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P43" s="37" t="s">
-        <v>306</v>
+      <c r="P43" s="15" t="s">
+        <v>305</v>
       </c>
       <c r="Q43" s="15"/>
       <c r="R43" s="16"/>
@@ -3847,8 +3852,8 @@
       <c r="O44" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P44" s="37" t="s">
-        <v>306</v>
+      <c r="P44" s="15" t="s">
+        <v>305</v>
       </c>
       <c r="Q44" s="15"/>
       <c r="R44" s="16"/>
@@ -3901,8 +3906,8 @@
       <c r="O45" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P45" s="37" t="s">
-        <v>306</v>
+      <c r="P45" s="15" t="s">
+        <v>305</v>
       </c>
       <c r="Q45" s="15"/>
       <c r="R45" s="16"/>
@@ -3955,8 +3960,8 @@
       <c r="O46" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P46" s="37" t="s">
-        <v>306</v>
+      <c r="P46" s="15" t="s">
+        <v>305</v>
       </c>
       <c r="Q46" s="15"/>
       <c r="R46" s="16"/>
@@ -4009,8 +4014,8 @@
       <c r="O47" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P47" s="37" t="s">
-        <v>306</v>
+      <c r="P47" s="15" t="s">
+        <v>305</v>
       </c>
       <c r="Q47" s="15"/>
       <c r="R47" s="16"/>
@@ -4063,8 +4068,8 @@
       <c r="O48" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P48" s="37" t="s">
-        <v>306</v>
+      <c r="P48" s="15" t="s">
+        <v>305</v>
       </c>
       <c r="Q48" s="15"/>
       <c r="R48" s="16"/>
@@ -4117,8 +4122,8 @@
       <c r="O49" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P49" s="37" t="s">
-        <v>306</v>
+      <c r="P49" s="15" t="s">
+        <v>305</v>
       </c>
       <c r="Q49" s="15"/>
       <c r="R49" s="16"/>
@@ -4171,8 +4176,8 @@
       <c r="O50" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P50" s="37" t="s">
-        <v>306</v>
+      <c r="P50" s="15" t="s">
+        <v>305</v>
       </c>
       <c r="Q50" s="15"/>
       <c r="R50" s="16"/>
@@ -4225,8 +4230,8 @@
       <c r="O51" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P51" s="37" t="s">
-        <v>306</v>
+      <c r="P51" s="15" t="s">
+        <v>305</v>
       </c>
       <c r="Q51" s="15"/>
       <c r="R51" s="16"/>
@@ -4279,8 +4284,8 @@
       <c r="O52" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P52" s="37" t="s">
-        <v>306</v>
+      <c r="P52" s="15" t="s">
+        <v>305</v>
       </c>
       <c r="Q52" s="15"/>
       <c r="R52" s="16"/>
@@ -4333,8 +4338,8 @@
       <c r="O53" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P53" s="37" t="s">
-        <v>306</v>
+      <c r="P53" s="15" t="s">
+        <v>305</v>
       </c>
       <c r="Q53" s="15"/>
       <c r="R53" s="16"/>
@@ -4387,8 +4392,8 @@
       <c r="O54" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P54" s="37" t="s">
-        <v>306</v>
+      <c r="P54" s="15" t="s">
+        <v>305</v>
       </c>
       <c r="Q54" s="15"/>
       <c r="R54" s="16"/>
@@ -4441,8 +4446,8 @@
       <c r="O55" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P55" s="37" t="s">
-        <v>306</v>
+      <c r="P55" s="15" t="s">
+        <v>305</v>
       </c>
       <c r="Q55" s="15"/>
       <c r="R55" s="16"/>
@@ -4495,8 +4500,8 @@
       <c r="O56" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P56" s="37" t="s">
-        <v>306</v>
+      <c r="P56" s="15" t="s">
+        <v>305</v>
       </c>
       <c r="Q56" s="15"/>
       <c r="R56" s="16"/>
@@ -4549,8 +4554,8 @@
       <c r="O57" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P57" s="37" t="s">
-        <v>306</v>
+      <c r="P57" s="15" t="s">
+        <v>305</v>
       </c>
       <c r="Q57" s="15"/>
       <c r="R57" s="16"/>
@@ -4603,8 +4608,8 @@
       <c r="O58" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P58" s="37" t="s">
-        <v>306</v>
+      <c r="P58" s="15" t="s">
+        <v>305</v>
       </c>
       <c r="Q58" s="15"/>
       <c r="R58" s="16"/>
@@ -4657,8 +4662,8 @@
       <c r="O59" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P59" s="37" t="s">
-        <v>306</v>
+      <c r="P59" s="15" t="s">
+        <v>305</v>
       </c>
       <c r="Q59" s="15"/>
       <c r="R59" s="16"/>
@@ -4711,8 +4716,8 @@
       <c r="O60" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="P60" s="37" t="s">
-        <v>306</v>
+      <c r="P60" s="15" t="s">
+        <v>305</v>
       </c>
       <c r="Q60" s="15"/>
       <c r="R60" s="16"/>

</xml_diff>